<commit_message>
works without the date
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +745,510 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:22:02</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>16:22:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:22:34</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>16:22:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:23:05</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>16:23:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:23:36</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>16:23:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:24:07</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>16:24:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:24:39</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:26:19</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label-wrapper button[aria-label*='30']"}
+  (Session info: chrome=128.0.6613.120); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF7F082B5D2+29090]
+	(No symbol) [0x00007FF7F079E689]
+	(No symbol) [0x00007FF7F065B1CA]
+	(No symbol) [0x00007FF7F06AEFD7]
+	(No symbol) [0x00007FF7F06AF22C]
+	(No symbol) [0x00007FF7F06F97F7]
+	(No symbol) [0x00007FF7F06D672F]
+	(No symbol) [0x00007FF7F06F65D9]
+	(No symbol) [0x00007FF7F06D6493]
+	(No symbol) [0x00007FF7F06A09B1]
+	(No symbol) [0x00007FF7F06A1B11]
+	GetHandleVerifier [0x00007FF7F0B48C5D+3295277]
+	GetHandleVerifier [0x00007FF7F0B94843+3605523]
+	GetHandleVerifier [0x00007FF7F0B8A707+3564247]
+	GetHandleVerifier [0x00007FF7F08E6EB6+797318]
+	(No symbol) [0x00007FF7F07A980F]
+	(No symbol) [0x00007FF7F07A53F4]
+	(No symbol) [0x00007FF7F07A5580]
+	(No symbol) [0x00007FF7F0794A1F]
+	BaseThreadInitThunk [0x00007FFC979C257D+29]
+	RtlUserThreadStart [0x00007FFC9896AF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>16:26:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:33:12</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>16:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:33:44</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>16:33:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:43:45</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>16:43:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:44:17</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>16:44:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:51:07</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>16:51:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:51:33</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>16:51:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:51:54</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>16:51:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:52:35</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>16:52:35</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
starting with BCE Structure again
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1281,6 +1281,70 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-09-12 18:32:12</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>18:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-09-12 18:34:16</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>MOCKURL_https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>MOCK_No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>18:34:16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Basic things with correct structutre
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1345,6 +1345,70 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-09-12 19:36:57</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>MOCKURL_https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>MOCK_No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>19:36:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-09-12 19:42:53</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>MOCKURL_https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>MOCK_No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>19:42:53</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
everything should be good
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,6 +593,102 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-09-22 23:48:05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/the-rux-nashville</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-09-22</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>23:48:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-09-22 23:48:58</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/the-rux-nashville</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-09-22</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>23:48:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-09-22 23:49:21</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/the-rux-nashville</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-09-22</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>23:49:21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update in the parsing
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -969,6 +969,62 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-09-23 17:03:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=128.0.6613.138); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF7BD199412+29090]
+	(No symbol) [0x00007FF7BD10E239]
+	(No symbol) [0x00007FF7BCFCB1DA]
+	(No symbol) [0x00007FF7BD01EFE7]
+	(No symbol) [0x00007FF7BD01F23C]
+	(No symbol) [0x00007FF7BD0697C7]
+	(No symbol) [0x00007FF7BD04672F]
+	(No symbol) [0x00007FF7BD0665A2]
+	(No symbol) [0x00007FF7BD046493]
+	(No symbol) [0x00007FF7BD0109D1]
+	(No symbol) [0x00007FF7BD011B31]
+	GetHandleVerifier [0x00007FF7BD4B871D+3302573]
+	GetHandleVerifier [0x00007FF7BD504243+3612627]
+	GetHandleVerifier [0x00007FF7BD4FA417+3572135]
+	GetHandleVerifier [0x00007FF7BD255EB6+801862]
+	(No symbol) [0x00007FF7BD11945F]
+	(No symbol) [0x00007FF7BD114FB4]
+	(No symbol) [0x00007FF7BD115140]
+	(No symbol) [0x00007FF7BD10461F]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>17:03:50</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
workıng at some poınt
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1025,6 +1025,878 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:48:34</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>18:48:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:49:54</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>18:49:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:50:19</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>18:50:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:50:32</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>18:50:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:50:43</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>18:50:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:50:50</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>18:50:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:51:07</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>18:51:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:51:10</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>18:51:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:56:06</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-wrapper button[aria-label*='september 27']"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>18:56:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:57:57</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>18:57:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:58:18</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>18:58:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-09-23 18:58:38</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>18:58:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-09-23 19:00:45</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>19:00:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-09-23 19:01:04</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>19:01:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-09-23 19:01:24</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>19:01:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-09-23 19:01:44</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.59); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF6705EFDA5+29557]
+	(No symbol) [0x00007FF670562240]
+	(No symbol) [0x00007FF67041B6EA]
+	(No symbol) [0x00007FF67046FA15]
+	(No symbol) [0x00007FF67046FC6C]
+	(No symbol) [0x00007FF6704BBB07]
+	(No symbol) [0x00007FF67049753F]
+	(No symbol) [0x00007FF6704B88A3]
+	(No symbol) [0x00007FF6704972A3]
+	(No symbol) [0x00007FF6704612DF]
+	(No symbol) [0x00007FF670462451]
+	GetHandleVerifier [0x00007FF67091DCBD+3363469]
+	GetHandleVerifier [0x00007FF670969B47+3674391]
+	GetHandleVerifier [0x00007FF67095EAEB+3629243]
+	GetHandleVerifier [0x00007FF6706AFC66+815670]
+	(No symbol) [0x00007FF67056D6EF]
+	(No symbol) [0x00007FF6705692B4]
+	(No symbol) [0x00007FF670569450]
+	(No symbol) [0x00007FF6705581FF]
+	BaseThreadInitThunk [0x00007FFAEA46257D+29]
+	RtlUserThreadStart [0x00007FFAEB4EAF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>19:01:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-09-23 19:07:53</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date September 27 is available for booking.</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>19:07:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-09-23 19:08:26</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date September 27 is available for booking.</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>19:08:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-09-23 19:10:04</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Checked availability: Unable to determine availability. Please try again.</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>19:10:04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
price and availability tests passed
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2514,6 +2514,1894 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:34:51</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>02:34:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:34:51</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>02:34:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:34:51</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>02:34:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:36:03</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>02:36:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:36:04</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>02:36:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:36:04</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>02:36:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:39:23</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>02:39:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:39:29</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>02:39:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:39:34</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>02:39:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:39:39</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>02:39:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:39:53</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>02:39:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:39:59</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>02:39:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:04</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>02:40:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:09</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>02:40:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:14</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>02:40:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:19</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>02:40:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:24</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>02:40:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:29</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>02:40:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:34</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>02:40:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:39</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>02:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:44</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>02:40:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:40:49</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>02:40:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:43:03</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>02:43:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:43:33</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>02:43:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:43:34</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>02:43:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:44:39</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>02:44:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:44:41</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>02:44:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:46:23</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>02:46:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:48:16</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>02:48:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:49:04</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>02:49:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:49:05</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>02:49:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:49:10</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>02:49:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:49:15</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>02:49:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:49:20</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>02:49:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:50:07</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>02:50:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:50:09</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>02:50:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:52:02</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>02:52:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:52:03</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Checked availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>02:52:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:53:09</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>02:53:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:53:10</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Checked availability: S</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>02:53:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:54:26</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>02:54:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:54:29</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Checked availability: S</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>02:54:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:55:07</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Checked availability: S</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>02:55:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:55:09</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>02:55:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:58:08</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>02:58:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:58:10</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>02:58:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:58:49</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>02:58:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-09-29 02:58:50</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>02:58:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:00:23</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>03:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:00:24</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>03:00:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:01:30</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>03:01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:01:31</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>03:01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:02:31</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>03:02:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:02:33</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>03:02:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:27:28</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>03:27:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:27:29</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>03:27:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:27:29</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>03:27:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:27:34</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>03:27:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:27:35</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>03:27:35</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
all tests are done
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4402,6 +4402,966 @@
         </is>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:28:40</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>03:28:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:28:40</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>03:28:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:28:40</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>03:28:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:28:41</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>03:28:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:28:42</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>03:28:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:32:53</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>03:32:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:32:53</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>03:32:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:32:53</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>03:32:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:32:54</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>03:32:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:32:55</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>03:32:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:48:55</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>03:48:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:48:55</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>03:48:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:48:55</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>03:48:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:48:56</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>03:48:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:48:57</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>03:48:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:49:42</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>03:49:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:49:42</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>03:49:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:49:42</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>03:49:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:49:43</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>03:49:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:49:44</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>03:49:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:52:26</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>03:52:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:52:26</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>03:52:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:52:26</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>03:52:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:52:27</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>03:52:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:52:28</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>03:52:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:53:02</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>03:53:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:53:02</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>03:53:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:53:03</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>03:53:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:53:03</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>03:53:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:53:04</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>03:53:04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
everything is updated not tested
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5362,6 +5362,326 @@
         </is>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:54:47</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>03:54:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:54:47</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>03:54:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:54:47</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>03:54:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:54:48</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>03:54:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:54:49</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>03:54:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:56:04</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>03:56:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:56:05</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>03:56:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:56:05</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>03:56:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:56:05</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>03:56:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2024-09-29 03:56:06</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>03:56:06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
working on add account
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F221"/>
+  <dimension ref="A1:F239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8082,6 +8082,582 @@
         </is>
       </c>
     </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:51:30</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>21:51:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:51:31</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>21:51:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:51:31</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>21:51:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:51:31</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>21:51:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:51:33</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>21:51:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:54:06</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>21:54:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:54:07</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>21:54:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:54:07</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>21:54:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:54:07</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>21:54:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2024-09-30 21:54:09</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>21:54:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2024-09-30 22:04:35</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>22:04:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2024-09-30 22:04:36</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>22:04:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2024-09-30 22:04:36</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>22:04:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2024-09-30 22:07:52</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>22:07:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2024-09-30 22:07:52</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>22:07:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2024-09-30 22:07:52</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>22:07:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2024-09-30 22:07:53</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>22:07:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2024-09-30 22:07:54</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>22:07:54</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data export moved to control and works
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F239"/>
+  <dimension ref="A1:F248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8658,6 +8658,438 @@
         </is>
       </c>
     </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:33:16</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>https://www.bestbuy.com/site/microsoft-xbox-wireless-controller-for-xbox-series-x-xbox-series-s-xbox-one-windows-devices-sky-cipher-special-edition/6584960.p?skuId=6584960</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>$69.99</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>20:33:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:33:22</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>https://www.bestbuy.com/site/microsoft-xbox-wireless-controller-for-xbox-series-x-xbox-series-s-xbox-one-windows-devices-sky-cipher-special-edition/6584960.p?skuId=6584960</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>$69.99</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>20:33:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:33:59</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/the-rux-nashville</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>20:33:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:34:04</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.71); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF60823B645+29573]
+	(No symbol) [0x00007FF6081B0470]
+	(No symbol) [0x00007FF60806B6EA]
+	(No symbol) [0x00007FF6080BF815]
+	(No symbol) [0x00007FF6080BFA6C]
+	(No symbol) [0x00007FF60810B917]
+	(No symbol) [0x00007FF6080E733F]
+	(No symbol) [0x00007FF6081086BC]
+	(No symbol) [0x00007FF6080E70A3]
+	(No symbol) [0x00007FF6080B12DF]
+	(No symbol) [0x00007FF6080B2441]
+	GetHandleVerifier [0x00007FF60856C58D+3375821]
+	GetHandleVerifier [0x00007FF6085B7987+3684039]
+	GetHandleVerifier [0x00007FF6085ACDAB+3640043]
+	GetHandleVerifier [0x00007FF6082FB7C6+816390]
+	(No symbol) [0x00007FF6081BB77F]
+	(No symbol) [0x00007FF6081B75A4]
+	(No symbol) [0x00007FF6081B7740]
+	(No symbol) [0x00007FF6081A659F]
+	BaseThreadInitThunk [0x00007FFF5DA8257D+29]
+	RtlUserThreadStart [0x00007FFF5ECEAF08+40]
+</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>20:34:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:34:23</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.71); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF60823B645+29573]
+	(No symbol) [0x00007FF6081B0470]
+	(No symbol) [0x00007FF60806B6EA]
+	(No symbol) [0x00007FF6080BF815]
+	(No symbol) [0x00007FF6080BFA6C]
+	(No symbol) [0x00007FF60810B917]
+	(No symbol) [0x00007FF6080E733F]
+	(No symbol) [0x00007FF6081086BC]
+	(No symbol) [0x00007FF6080E70A3]
+	(No symbol) [0x00007FF6080B12DF]
+	(No symbol) [0x00007FF6080B2441]
+	GetHandleVerifier [0x00007FF60856C58D+3375821]
+	GetHandleVerifier [0x00007FF6085B7987+3684039]
+	GetHandleVerifier [0x00007FF6085ACDAB+3640043]
+	GetHandleVerifier [0x00007FF6082FB7C6+816390]
+	(No symbol) [0x00007FF6081BB77F]
+	(No symbol) [0x00007FF6081B75A4]
+	(No symbol) [0x00007FF6081B7740]
+	(No symbol) [0x00007FF6081A659F]
+	BaseThreadInitThunk [0x00007FFF5DA8257D+29]
+	RtlUserThreadStart [0x00007FFF5ECEAF08+40]
+</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>20:34:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:34:41</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/hals-the-steakhouse-nashville</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.71); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF60823B645+29573]
+	(No symbol) [0x00007FF6081B0470]
+	(No symbol) [0x00007FF60806B6EA]
+	(No symbol) [0x00007FF6080BF815]
+	(No symbol) [0x00007FF6080BFA6C]
+	(No symbol) [0x00007FF60810B917]
+	(No symbol) [0x00007FF6080E733F]
+	(No symbol) [0x00007FF6081086BC]
+	(No symbol) [0x00007FF6080E70A3]
+	(No symbol) [0x00007FF6080B12DF]
+	(No symbol) [0x00007FF6080B2441]
+	GetHandleVerifier [0x00007FF60856C58D+3375821]
+	GetHandleVerifier [0x00007FF6085B7987+3684039]
+	GetHandleVerifier [0x00007FF6085ACDAB+3640043]
+	GetHandleVerifier [0x00007FF6082FB7C6+816390]
+	(No symbol) [0x00007FF6081BB77F]
+	(No symbol) [0x00007FF6081B75A4]
+	(No symbol) [0x00007FF6081B7740]
+	(No symbol) [0x00007FF6081A659F]
+	BaseThreadInitThunk [0x00007FFF5DA8257D+29]
+	RtlUserThreadStart [0x00007FFF5ECEAF08+40]
+</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>20:34:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:35:06</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/sinatra-bar-and-lounge-nashville</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.71); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF60823B645+29573]
+	(No symbol) [0x00007FF6081B0470]
+	(No symbol) [0x00007FF60806B6EA]
+	(No symbol) [0x00007FF6080BF815]
+	(No symbol) [0x00007FF6080BFA6C]
+	(No symbol) [0x00007FF60810B917]
+	(No symbol) [0x00007FF6080E733F]
+	(No symbol) [0x00007FF6081086BC]
+	(No symbol) [0x00007FF6080E70A3]
+	(No symbol) [0x00007FF6080B12DF]
+	(No symbol) [0x00007FF6080B2441]
+	GetHandleVerifier [0x00007FF60856C58D+3375821]
+	GetHandleVerifier [0x00007FF6085B7987+3684039]
+	GetHandleVerifier [0x00007FF6085ACDAB+3640043]
+	GetHandleVerifier [0x00007FF6082FB7C6+816390]
+	(No symbol) [0x00007FF6081BB77F]
+	(No symbol) [0x00007FF6081B75A4]
+	(No symbol) [0x00007FF6081B7740]
+	(No symbol) [0x00007FF6081A659F]
+	BaseThreadInitThunk [0x00007FFF5DA8257D+29]
+	RtlUserThreadStart [0x00007FFF5ECEAF08+40]
+</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>20:35:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:35:25</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/sinatra-bar-and-lounge-nashville</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.71); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF60823B645+29573]
+	(No symbol) [0x00007FF6081B0470]
+	(No symbol) [0x00007FF60806B6EA]
+	(No symbol) [0x00007FF6080BF815]
+	(No symbol) [0x00007FF6080BFA6C]
+	(No symbol) [0x00007FF60810B917]
+	(No symbol) [0x00007FF6080E733F]
+	(No symbol) [0x00007FF6081086BC]
+	(No symbol) [0x00007FF6080E70A3]
+	(No symbol) [0x00007FF6080B12DF]
+	(No symbol) [0x00007FF6080B2441]
+	GetHandleVerifier [0x00007FF60856C58D+3375821]
+	GetHandleVerifier [0x00007FF6085B7987+3684039]
+	GetHandleVerifier [0x00007FF6085ACDAB+3640043]
+	GetHandleVerifier [0x00007FF6082FB7C6+816390]
+	(No symbol) [0x00007FF6081BB77F]
+	(No symbol) [0x00007FF6081B75A4]
+	(No symbol) [0x00007FF6081B7740]
+	(No symbol) [0x00007FF6081A659F]
+	BaseThreadInitThunk [0x00007FFF5DA8257D+29]
+	RtlUserThreadStart [0x00007FFF5ECEAF08+40]
+</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>20:35:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:35:43</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/sinatra-bar-and-lounge-nashville</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checked availability: Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label"}
+  (Session info: chrome=129.0.6668.71); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF60823B645+29573]
+	(No symbol) [0x00007FF6081B0470]
+	(No symbol) [0x00007FF60806B6EA]
+	(No symbol) [0x00007FF6080BF815]
+	(No symbol) [0x00007FF6080BFA6C]
+	(No symbol) [0x00007FF60810B917]
+	(No symbol) [0x00007FF6080E733F]
+	(No symbol) [0x00007FF6081086BC]
+	(No symbol) [0x00007FF6080E70A3]
+	(No symbol) [0x00007FF6080B12DF]
+	(No symbol) [0x00007FF6080B2441]
+	GetHandleVerifier [0x00007FF60856C58D+3375821]
+	GetHandleVerifier [0x00007FF6085B7987+3684039]
+	GetHandleVerifier [0x00007FF6085ACDAB+3640043]
+	GetHandleVerifier [0x00007FF6082FB7C6+816390]
+	(No symbol) [0x00007FF6081BB77F]
+	(No symbol) [0x00007FF6081B75A4]
+	(No symbol) [0x00007FF6081B7740]
+	(No symbol) [0x00007FF6081A659F]
+	BaseThreadInitThunk [0x00007FFF5DA8257D+29]
+	RtlUserThreadStart [0x00007FFF5ECEAF08+40]
+</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data Export unit test completed
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F248"/>
+  <dimension ref="A1:F256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9090,6 +9090,262 @@
         </is>
       </c>
     </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:10:52</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>21:10:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:10:52</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>21:10:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:10:52</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>21:10:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:10:52</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>https://example.com/product</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>$199.99</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>21:10:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:10:53</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>invalid_url</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Error fetching price: Invalid URL</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>21:10:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:10:53</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>21:10:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:10:54</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>21:10:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:10:55</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>https://example.com/product</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>100 USD</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>21:10:55</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
config added, pdfs updated
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F256"/>
+  <dimension ref="A1:F258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9346,6 +9346,70 @@
         </is>
       </c>
     </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:41:40</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>https://www.bestbuy.com/site/microsoft-xbox-wireless-controller-for-xbox-series-x-xbox-series-s-xbox-one-windows-devices-sky-cipher-special-edition/6584960.p?skuId=6584960</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>$69.99</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>21:41:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2024-10-01 21:41:58</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>https://www.bestbuy.com/site/microsoft-xbox-wireless-controller-for-xbox-series-x-xbox-series-s-xbox-one-windows-devices-sky-cipher-special-edition/6584960.p?skuId=6584960</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>$69.99</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>21:41:58</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
push recent changes and test and assignments
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F272"/>
+  <dimension ref="A1:F283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9858,6 +9858,358 @@
         </is>
       </c>
     </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2024-10-02 16:54:42</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>16:54:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2024-10-02 17:15:04</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>17:15:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2024-10-02 17:15:04</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>17:15:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2024-10-02 17:15:04</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>17:15:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2024-10-02 17:15:05</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>https://example.com/product</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>$199.99</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>17:15:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2024-10-02 17:15:05</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>invalid_url</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Error fetching price: Invalid URL</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>17:15:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2024-10-02 17:15:05</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>17:15:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2024-10-02 17:15:06</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>17:15:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2024-10-02 17:15:07</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>https://example.com/product</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>100 USD</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>17:15:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2024-10-02 18:03:26</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>https://example.com/product</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>100 USD</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>18:03:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2024-10-02 18:03:55</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>https://example.com/product</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>100 USD</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>2024-10-02</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>18:03:55</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
working on uniot test
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F325"/>
+  <dimension ref="A1:F330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11578,6 +11578,166 @@
         </is>
       </c>
     </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>2024-10-08 12:16:31</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date current date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>12:16:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>2024-10-08 12:16:32</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>12:16:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>2024-10-08 12:16:32</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Checked availability: No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>12:16:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>2024-10-08 12:16:33</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Checked availability: Selected or default date is available for booking.</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>12:16:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>2024-10-08 12:16:34</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://example.com</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Failed to check availability: Failed to check availability</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>12:16:34</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
tests organized and passed
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F338"/>
+  <dimension ref="A1:F342"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11994,6 +11994,134 @@
         </is>
       </c>
     </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2024-10-08 21:15:41</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://example.com/reservation</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Checked availability: ('Checked availability: Availability confirmed', 'Data saved to Excel file at ExportedFiles\\excelFiles\\check_availability.xlsx.', 'HTML file saved and updated at ExportedFiles\\htmlFiles\\check_availability.html.')</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>21:15:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2024-10-08 21:18:32</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://example.com/reservation</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Checked availability: ('Checked availability: Availability confirmed', 'Data saved to Excel file at ExportedFiles\\excelFiles\\check_availability.xlsx.', 'HTML file saved and updated at ExportedFiles\\htmlFiles\\check_availability.html.')</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>21:18:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>2024-10-08 21:21:53</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://example.com/reservation</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>Checked availability: ('Checked availability: Availability confirmed', 'Data saved to Excel file at ExportedFiles\\excelFiles\\check_availability.xlsx.', 'HTML file saved and updated at ExportedFiles\\htmlFiles\\check_availability.html.')</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>21:21:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>2024-10-08 21:24:54</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://example.com/reservation</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>Checked availability: ('Checked availability: Availability confirmed', 'Data saved to Excel file at ExportedFiles\\excelFiles\\check_availability.xlsx.', 'HTML file saved and updated at ExportedFiles\\htmlFiles\\check_availability.html.')</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>21:24:54</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
save files before losing
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F344"/>
+  <dimension ref="A1:F345"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12186,6 +12186,38 @@
         </is>
       </c>
     </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>2024-10-09 11:22:42</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://example.com/reservation</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Checked availability: ('Checked availability: Availability confirmed', 'Data saved to Excel file at ExportedFiles\\excelFiles\\check_availability.xlsx.', 'HTML file saved and updated at ExportedFiles\\htmlFiles\\check_availability.html.')</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>2024-10-09</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>11:22:42</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
only fixed get price
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F345"/>
+  <dimension ref="A1:F346"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12218,6 +12218,38 @@
         </is>
       </c>
     </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>2024-10-09 14:22:04</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://example.com/reservation</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Checked availability: ('Checked availability: Availability confirmed', 'Data saved to Excel file at ExportedFiles\\excelFiles\\check_availability.xlsx.', 'HTML file saved and updated at ExportedFiles\\htmlFiles\\check_availability.html.')</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>2024-10-09</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>14:22:04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chapter and assignment updates
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F346"/>
+  <dimension ref="A1:F347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12250,6 +12250,38 @@
         </is>
       </c>
     </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>2024-10-09 14:29:18</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://example.com/reservation</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Checked availability: ('Checked availability: Availability confirmed', 'Data saved to Excel file at ExportedFiles\\excelFiles\\check_availability.xlsx.', 'HTML file saved and updated at ExportedFiles\\htmlFiles\\check_availability.html.')</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>2024-10-09</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>14:29:18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
clean up and recent changes
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/check_availability.xlsx
+++ b/ExportedFiles/excelFiles/check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F347"/>
+  <dimension ref="A1:F348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12282,6 +12282,38 @@
         </is>
       </c>
     </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>2024-10-09 23:31:35</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://example.com/reservation</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>Checked availability: ('Checked availability: Availability confirmed', 'Data saved to Excel file at ExportedFiles\\excelFiles\\check_availability.xlsx.', 'HTML file saved and updated at ExportedFiles\\htmlFiles\\check_availability.html.')</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>2024-10-09</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>23:31:35</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>